<commit_message>
Started with player search functionality
</commit_message>
<xml_diff>
--- a/database_design.xlsx
+++ b/database_design.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stijn\Documents\Unity\cyvasse\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
   <si>
     <t>Main Structure</t>
   </si>
@@ -241,6 +246,27 @@
   </si>
   <si>
     <t>***** saving 1 field per unit means less rows &amp; quicker loading times (board = 91 rows, units = 52 rows) -&gt; ONLY WORKS if you have a max per unit!!!</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Create Account</t>
+  </si>
+  <si>
+    <t>Search player</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Create game</t>
+  </si>
+  <si>
+    <t>Accept game</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -248,7 +274,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -464,7 +490,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -503,12 +529,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,6 +558,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency 2" xfId="2"/>
@@ -549,6 +575,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -597,7 +626,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -632,7 +661,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -843,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15"/>
@@ -860,22 +889,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
     </row>
@@ -887,7 +916,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="30"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -915,18 +944,18 @@
         <v>22</v>
       </c>
       <c r="J3" s="9"/>
-      <c r="K3" s="36">
+      <c r="K3" s="34">
         <v>6</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="43" t="s">
+      <c r="M3" s="33"/>
+      <c r="N3" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="34" t="s">
+      <c r="O3" s="34"/>
+      <c r="P3" s="32" t="s">
         <v>49</v>
       </c>
     </row>
@@ -939,29 +968,29 @@
         <v>9</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="43" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="35" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="36">
+      <c r="K4" s="34">
         <v>1</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="41" t="s">
+      <c r="M4" s="33"/>
+      <c r="N4" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="34" t="s">
+      <c r="O4" s="34"/>
+      <c r="P4" s="32" t="s">
         <v>48</v>
       </c>
     </row>
@@ -974,10 +1003,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="29" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="16"/>
@@ -985,18 +1014,18 @@
         <v>3</v>
       </c>
       <c r="J5" s="9"/>
-      <c r="K5" s="36">
+      <c r="K5" s="34">
         <v>6</v>
       </c>
-      <c r="L5" s="41" t="s">
+      <c r="L5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="35"/>
-      <c r="N5" s="41" t="s">
+      <c r="M5" s="33"/>
+      <c r="N5" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="36"/>
-      <c r="P5" s="34" t="s">
+      <c r="O5" s="34"/>
+      <c r="P5" s="32" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1009,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="44" t="s">
         <v>63</v>
       </c>
       <c r="G6" s="19" t="s">
@@ -1020,18 +1049,18 @@
         <v>23</v>
       </c>
       <c r="J6" s="24"/>
-      <c r="K6" s="34">
+      <c r="K6" s="32">
         <v>2</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="38" t="s">
         <v>31</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="40" t="s">
+      <c r="N6" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34" t="s">
+      <c r="O6" s="32"/>
+      <c r="P6" s="32" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1044,7 +1073,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="44" t="s">
         <v>64</v>
       </c>
       <c r="G7" s="19" t="s">
@@ -1055,17 +1084,17 @@
         <v>24</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="K7" s="35">
+      <c r="K7" s="33">
         <v>2</v>
       </c>
-      <c r="L7" s="40" t="s">
+      <c r="L7" s="38" t="s">
         <v>32</v>
       </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="35"/>
+      <c r="O7" s="33"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16">
@@ -1073,11 +1102,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>55</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="44" t="s">
         <v>65</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -1088,17 +1117,17 @@
         <v>26</v>
       </c>
       <c r="J8" s="9"/>
-      <c r="K8" s="35">
+      <c r="K8" s="33">
         <v>2</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="L8" s="38" t="s">
         <v>33</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="40" t="s">
+      <c r="N8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="35"/>
+      <c r="O8" s="33"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16">
@@ -1110,24 +1139,24 @@
         <v>56</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="44" t="s">
         <v>66</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="1"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="35">
+      <c r="K9" s="33">
         <v>2</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="42" t="s">
         <v>34</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="44" t="s">
+      <c r="N9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="35"/>
+      <c r="O9" s="33"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16">
@@ -1135,122 +1164,122 @@
         <v>54</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="43" t="s">
         <v>58</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="44" t="s">
         <v>67</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="35">
+      <c r="K10" s="33">
         <v>2</v>
       </c>
-      <c r="L10" s="44" t="s">
+      <c r="L10" s="42" t="s">
         <v>35</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="44" t="s">
+      <c r="N10" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="O10" s="35"/>
+      <c r="O10" s="33"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="1"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="45" t="s">
         <v>69</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="23"/>
-      <c r="K11" s="48">
+      <c r="K11" s="46">
         <v>2</v>
       </c>
-      <c r="L11" s="44" t="s">
+      <c r="L11" s="42" t="s">
         <v>36</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="44" t="s">
+      <c r="N11" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="35"/>
+      <c r="O11" s="33"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="1"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="45" t="s">
         <v>70</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="38"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="12"/>
       <c r="K12" s="9">
         <v>1</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="L12" s="37" t="s">
         <v>37</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="39" t="s">
+      <c r="N12" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="35"/>
+      <c r="O12" s="33"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1"/>
       <c r="B13" s="9"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="47" t="s">
+      <c r="D13" s="33"/>
+      <c r="E13" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="35"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="38"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="O13" s="35"/>
+      <c r="O13" s="33"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="49" t="s">
+      <c r="D14" s="33"/>
+      <c r="E14" s="47" t="s">
         <v>73</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="38"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="10"/>
       <c r="K14" s="9">
         <f>K3+K4+K5+K6+K7+K8+K9+K10+K11+K12</f>
         <v>26</v>
       </c>
-      <c r="O14" s="35"/>
+      <c r="O14" s="33"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16">
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="50" t="s">
+      <c r="D15" s="33"/>
+      <c r="E15" s="48" t="s">
         <v>21</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="38"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="25"/>
       <c r="K15" s="15"/>
       <c r="O15" s="1"/>
@@ -1260,12 +1289,12 @@
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="30" t="s">
         <v>59</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="38"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="25"/>
       <c r="K16" s="15"/>
       <c r="O16" s="1"/>
@@ -1275,12 +1304,12 @@
       <c r="B17" s="1"/>
       <c r="C17" s="26"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="30" t="s">
         <v>60</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="38"/>
+      <c r="I17" s="36"/>
       <c r="J17" s="24"/>
       <c r="K17" s="1"/>
       <c r="O17" s="1"/>
@@ -1289,7 +1318,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="15"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="30" t="s">
         <v>61</v>
       </c>
       <c r="F18" s="1"/>
@@ -1299,7 +1328,7 @@
       <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>62</v>
       </c>
       <c r="H19" s="24"/>
@@ -1307,7 +1336,7 @@
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="30" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="24"/>
@@ -1322,25 +1351,25 @@
     <row r="22" spans="1:15">
       <c r="H22" s="24"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="34"/>
+      <c r="J22" s="32"/>
       <c r="K22" s="1"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="30"/>
       <c r="H23" s="24"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="34"/>
+      <c r="J23" s="32"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="24"/>
@@ -1362,7 +1391,7 @@
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="40" t="s">
         <v>25</v>
       </c>
       <c r="H26" s="24"/>
@@ -1373,7 +1402,7 @@
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="32" t="s">
         <v>74</v>
       </c>
       <c r="B27" s="1"/>
@@ -1416,12 +1445,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C12:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="3:7">
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7">
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7">
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Game UI listing, Split up managers, board data setup
</commit_message>
<xml_diff>
--- a/database_design.xlsx
+++ b/database_design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
   <si>
     <t>Main Structure</t>
   </si>
@@ -66,9 +66,6 @@
     <t>email (use as login)</t>
   </si>
   <si>
-    <t>accepted</t>
-  </si>
-  <si>
     <t>** player 1 is always the challenger</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>field_unit_3_0</t>
   </si>
   <si>
-    <t>***** saving 1 field per unit means less rows &amp; quicker loading times (board = 91 rows, units = 52 rows) -&gt; ONLY WORKS if you have a max per unit!!!</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
     <t>Create game</t>
   </si>
   <si>
-    <t>Accept game</t>
-  </si>
-  <si>
     <t>Logout</t>
   </si>
   <si>
@@ -262,6 +253,93 @@
   </si>
   <si>
     <t>player_black_id</t>
+  </si>
+  <si>
+    <t>1st move = accept</t>
+  </si>
+  <si>
+    <t>GetGames</t>
+  </si>
+  <si>
+    <t>naam tegenstander</t>
+  </si>
+  <si>
+    <t>0 = jou beurt, 1 andere beurt, 2 gedaan</t>
+  </si>
+  <si>
+    <t>0 = mislukt, 1 = gelukt</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>boards</t>
+  </si>
+  <si>
+    <t>board_layout</t>
+  </si>
+  <si>
+    <t>1 string per board</t>
+  </si>
+  <si>
+    <t>means all moves &amp; boards in 1 table = WAY SMALLER</t>
+  </si>
+  <si>
+    <t>eerste = unit type</t>
+  </si>
+  <si>
+    <t>tweede = unit id</t>
+  </si>
+  <si>
+    <t>derde = vak</t>
+  </si>
+  <si>
+    <t>xyzzz</t>
+  </si>
+  <si>
+    <t>5 * aantal units</t>
+  </si>
+  <si>
+    <t>260 bytes</t>
+  </si>
+  <si>
+    <t>***** saving 1 field per unit means less rows &amp; quicker loading times (board = 91 rows, units = 52 rows) -&gt; ONLY WORKS if you have a max per unit!!! -&gt; Werkt dus niet bij schaak maar wel bij cyvasse?</t>
+  </si>
+  <si>
+    <t>field_unit_2_2</t>
+  </si>
+  <si>
+    <t>field_unit_2_3</t>
+  </si>
+  <si>
+    <t>field_unit_2_4</t>
+  </si>
+  <si>
+    <t>field_unit_2_5</t>
+  </si>
+  <si>
+    <t>game_state******</t>
+  </si>
+  <si>
+    <t>****** 0 = setup, 1 = white turn, 2 = black turn, 3 = completed</t>
+  </si>
+  <si>
+    <t>field_fortress = 12</t>
+  </si>
+  <si>
+    <t>12/1/-1/...</t>
+  </si>
+  <si>
+    <t>Get games</t>
+  </si>
+  <si>
+    <t>Get specific game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; </t>
+  </si>
+  <si>
+    <t>bord vult</t>
   </si>
 </sst>
 </file>
@@ -271,7 +349,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,16 +452,54 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -487,7 +603,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -529,11 +645,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -545,7 +659,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -553,11 +667,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -865,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15"/>
@@ -884,22 +1010,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="28"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
     </row>
@@ -925,33 +1051,33 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="23"/>
-      <c r="I3" s="17" t="s">
-        <v>20</v>
+      <c r="I3" s="51" t="s">
+        <v>19</v>
       </c>
       <c r="J3" s="9"/>
-      <c r="K3" s="34">
+      <c r="K3" s="33">
         <v>6</v>
       </c>
-      <c r="L3" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="32" t="s">
-        <v>47</v>
+      <c r="L3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="32"/>
+      <c r="N3" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="33"/>
+      <c r="P3" s="31" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickTop="1">
@@ -963,30 +1089,30 @@
         <v>9</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="43" t="s">
-        <v>56</v>
+      <c r="E4" s="50" t="s">
+        <v>55</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="52" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="34">
+      <c r="K4" s="33">
         <v>1</v>
       </c>
-      <c r="L4" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="34"/>
-      <c r="P4" s="32" t="s">
-        <v>46</v>
+      <c r="L4" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="33"/>
+      <c r="P4" s="31" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -995,33 +1121,33 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="44" t="s">
-        <v>66</v>
+      <c r="E5" s="42" t="s">
+        <v>65</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="16"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="53" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="9"/>
-      <c r="K5" s="34">
+      <c r="K5" s="33">
         <v>6</v>
       </c>
-      <c r="L5" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="33"/>
-      <c r="N5" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" s="34"/>
-      <c r="P5" s="32" t="s">
-        <v>48</v>
+      <c r="L5" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="32"/>
+      <c r="N5" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="33"/>
+      <c r="P5" s="31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1030,33 +1156,33 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>11</v>
+      <c r="E6" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="9" t="s">
-        <v>21</v>
+      <c r="I6" s="53" t="s">
+        <v>20</v>
       </c>
       <c r="J6" s="24"/>
-      <c r="K6" s="32">
+      <c r="K6" s="31">
         <v>2</v>
       </c>
-      <c r="L6" s="38" t="s">
-        <v>29</v>
+      <c r="L6" s="36" t="s">
+        <v>28</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32" t="s">
-        <v>49</v>
+      <c r="N6" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1064,32 +1190,32 @@
         <v>15</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="43" t="s">
-        <v>56</v>
+      <c r="C7" s="50" t="s">
+        <v>55</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="44" t="s">
-        <v>62</v>
+      <c r="E7" s="42" t="s">
+        <v>61</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="2" t="s">
-        <v>22</v>
+      <c r="I7" s="54" t="s">
+        <v>21</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="K7" s="33">
+      <c r="K7" s="32">
         <v>2</v>
       </c>
-      <c r="L7" s="38" t="s">
-        <v>30</v>
+      <c r="L7" s="36" t="s">
+        <v>29</v>
       </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="O7" s="33"/>
+      <c r="N7" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="32"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16">
@@ -1097,336 +1223,468 @@
         <v>8</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="34" t="s">
-        <v>53</v>
+      <c r="C8" t="s">
+        <v>100</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>50</v>
+      <c r="E8" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>12</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="9" t="s">
-        <v>24</v>
+      <c r="I8" s="53" t="s">
+        <v>23</v>
       </c>
       <c r="J8" s="9"/>
-      <c r="K8" s="33">
+      <c r="K8" s="32">
         <v>2</v>
       </c>
-      <c r="L8" s="38" t="s">
-        <v>31</v>
+      <c r="L8" s="36" t="s">
+        <v>30</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="33"/>
+      <c r="N8" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" s="32"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" t="s">
-        <v>54</v>
+      <c r="C9" s="33" t="s">
+        <v>52</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="15"/>
+      <c r="E9" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="9"/>
+      <c r="I9" s="53"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="33">
+      <c r="K9" s="32">
         <v>2</v>
       </c>
-      <c r="L9" s="42" t="s">
-        <v>32</v>
+      <c r="L9" s="40" t="s">
+        <v>31</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="O9" s="33"/>
+      <c r="N9" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="32"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="19" t="s">
-        <v>16</v>
+      <c r="C10" t="s">
+        <v>53</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="44" t="s">
-        <v>65</v>
+      <c r="E10" s="42" t="s">
+        <v>64</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="55"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="33">
+      <c r="K10" s="32">
         <v>2</v>
       </c>
-      <c r="L10" s="42" t="s">
-        <v>33</v>
+      <c r="L10" s="40" t="s">
+        <v>32</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="33"/>
+      <c r="N10" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="32"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="45" t="s">
-        <v>67</v>
+      <c r="E11" s="43" t="s">
+        <v>66</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="23"/>
-      <c r="K11" s="46">
+      <c r="K11" s="44">
         <v>2</v>
       </c>
-      <c r="L11" s="42" t="s">
-        <v>34</v>
+      <c r="L11" s="40" t="s">
+        <v>33</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="O11" s="33"/>
+      <c r="N11" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="32"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="1"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="45" t="s">
-        <v>68</v>
+      <c r="E12" s="43" t="s">
+        <v>67</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="36"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="12"/>
       <c r="K12" s="9">
         <v>1</v>
       </c>
-      <c r="L12" s="37" t="s">
-        <v>35</v>
+      <c r="L12" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="O12" s="33"/>
+      <c r="N12" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="32"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1"/>
       <c r="B13" s="9"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="33"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="32"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="36"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="O13" s="33"/>
+      <c r="O13" s="32"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="19"/>
+      <c r="B14" s="9"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="32"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="36"/>
+      <c r="I14" s="56"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="9">
+      <c r="K14" s="10"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1"/>
+      <c r="B15" s="9"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="9">
         <f>K3+K4+K5+K6+K7+K8+K9+K10+K11+K12</f>
         <v>26</v>
       </c>
-      <c r="O14" s="33"/>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="1"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="15"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="30" t="s">
+      <c r="O18" s="32"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="B19" s="1"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="15"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="15"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="B21" s="1"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="15"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="B17" s="1"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="30" t="s">
+      <c r="G21" s="9"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="B22" s="1"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="B18" s="1"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="1"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="E19" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="1"/>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="E20" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="1"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="H21" s="24"/>
-      <c r="I21" s="1"/>
-      <c r="M21" s="9"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="F22" s="1"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="24"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="30"/>
+    <row r="23" spans="1:16">
+      <c r="E23" s="30" t="s">
+        <v>59</v>
+      </c>
       <c r="H23" s="24"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="32" t="s">
-        <v>17</v>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="E24" s="30" t="s">
+        <v>18</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" t="s">
-        <v>25</v>
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="E25" s="30" t="s">
+        <v>102</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="40" t="s">
-        <v>23</v>
-      </c>
+      <c r="M25" s="9"/>
+    </row>
+    <row r="26" spans="1:16">
       <c r="H26" s="24"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="31"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="E27" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="30"/>
       <c r="H27" s="24"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="J27" s="31"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+    <row r="28" spans="1:16">
       <c r="H28" s="24"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="E29" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="24"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="E30" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="B31" s="1"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="1"/>
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="E33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="E37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="E38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="38" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1440,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C12:G14"/>
+  <dimension ref="C11:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1455,37 +1713,74 @@
     <col min="7" max="7" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="11" spans="3:7">
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="12" spans="3:7">
       <c r="C12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" t="s">
         <v>76</v>
-      </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7">
-      <c r="C13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="3:7">
       <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
         <v>75</v>
       </c>
-      <c r="D14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>77</v>
-      </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7">
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>